<commit_message>
change virus name to current H3/H1 and older H1
</commit_message>
<xml_diff>
--- a/IMV/IAVapp/2018-11-30_HI-titers.xlsx
+++ b/IMV/IAVapp/2018-11-30_HI-titers.xlsx
@@ -5,18 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/Home$/schmutz.stefan/Projects/Med_Kurs/IAV/2018/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/schmutz.stefan/Dropbox/GitHub/shiny-server/IMV/IAVapp/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="7600" yWindow="5420" windowWidth="14400" windowHeight="9660"/>
+    <workbookView xWindow="6260" yWindow="580" windowWidth="22500" windowHeight="20860"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$1</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$C$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$D$1</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$D$37</definedName>
   </definedNames>
   <calcPr calcId="145621" concurrentCalc="0"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="37">
   <si>
     <t>A/Brisbane/59/2007</t>
   </si>
@@ -130,6 +130,18 @@
   </si>
   <si>
     <t>18ygv</t>
+  </si>
+  <si>
+    <t>virus_strain</t>
+  </si>
+  <si>
+    <t>older H1</t>
+  </si>
+  <si>
+    <t>current H3</t>
+  </si>
+  <si>
+    <t>current H1</t>
   </si>
 </sst>
 </file>
@@ -664,919 +676,1164 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C82"/>
+  <dimension ref="A1:D82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.33203125" customWidth="1"/>
-    <col min="2" max="2" width="28.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.1640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.1640625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="B2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="B3" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="13">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D4" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C5" s="5">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="B5" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="15">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="6">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="B6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="B7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="13">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="5">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D8" s="15">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C9" s="5">
+      <c r="B9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D9" s="13">
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:3" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C10" s="7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="B10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" s="15">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C11" s="7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="B11" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D11" s="15">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" s="7">
+      <c r="B12" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D12" s="12">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:3" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C13" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="16">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C14" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D14" s="17">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C15" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D15" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B16" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="B16" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="18">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C17" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B18" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C18" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B19" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C19" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D19" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C20" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D20" s="14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B21" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C21" s="5">
+      <c r="B21" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D21" s="13">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B22" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C22" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="B22" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D22" s="12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B23" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C23" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D23" s="16">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C24" s="5">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="B24" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D24" s="15">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B25" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C25" s="7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="B25" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C25" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D25" s="19">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C26" s="7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="B26" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C26" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" s="13">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C27" s="7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
+      <c r="B27" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" s="15">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" s="2" customFormat="1" ht="21" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B28" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C28" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="B28" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D28" s="12">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B29" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C29" s="12">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="B29" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C30" s="13">
+      <c r="B30" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30" s="5">
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B31" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C31" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="B31" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" s="6">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B32" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C32" s="15">
+      <c r="B32" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" s="6">
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B33" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C33" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="B33" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C33" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B34" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C34" s="13">
+      <c r="B34" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D34" s="5">
         <v>20</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B35" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C35" s="15">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="B35" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D35" s="8">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B36" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C36" s="13">
+      <c r="B36" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" s="5">
         <v>20</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B37" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C37" s="15">
+      <c r="B37" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D37" s="6">
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B38" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C38" s="15">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="B38" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D38" s="9">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B39" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C39" s="12">
+      <c r="B39" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D39" s="7">
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B40" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C40" s="16">
+      <c r="B40" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D40" s="11">
         <v>80</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B41" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C41" s="17">
+      <c r="B41" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D41" s="10">
         <v>320</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B42" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C42" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="B42" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D42" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B43" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C43" s="18">
+      <c r="B43" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D43" s="9">
         <v>160</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B44" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C44" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="B44" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D44" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B45" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C45" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="B45" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D45" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B46" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C46" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="B46" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D46" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B47" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C47" s="14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="B47" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D47" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B48" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C48" s="13">
+      <c r="B48" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D48" s="5">
         <v>20</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B49" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C49" s="12">
+      <c r="B49" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D49" s="7">
         <v>10</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B50" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C50" s="16">
+      <c r="B50" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D50" s="11">
         <v>80</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B51" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C51" s="15">
+      <c r="B51" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D51" s="6">
         <v>40</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B52" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C52" s="19">
+      <c r="B52" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D52" s="8">
         <v>80</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B53" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C53" s="13">
+      <c r="B53" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D53" s="5">
         <v>20</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B54" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C54" s="15">
+      <c r="B54" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D54" s="6">
         <v>40</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B55" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C55" s="12">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="B55" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D55" s="5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B56" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C56" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="B56" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D56" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B57" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C57" s="5">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="B57" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D57" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="B58" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C58" s="6">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="B58" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D58" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B59" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C59" s="6">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="B59" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C59" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D59" s="5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B60" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C60" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="B60" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C60" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D60" s="6">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="B61" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C61" s="5">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="B61" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C61" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D61" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="B62" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C62" s="8">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="B62" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C62" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D62" s="5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B63" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C63" s="5">
+      <c r="B63" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D63" s="5">
         <v>20</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B64" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C64" s="6">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="65" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="B64" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D64" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B65" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C65" s="9">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="66" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="B65" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C65" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D65" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B66" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C66" s="7">
+      <c r="B66" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D66" s="7">
         <v>10</v>
       </c>
     </row>
-    <row r="67" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="B67" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C67" s="11">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="B67" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C67" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D67" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B68" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C68" s="10">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="B68" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D68" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B69" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C69" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="B69" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D69" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B70" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C70" s="9">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="71" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="B70" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C70" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D70" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B71" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C71" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="B71" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D71" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B72" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C72" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="B72" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C72" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D72" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B73" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C73" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="B73" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C73" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D73" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B74" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C74" s="4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="B74" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C74" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D74" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B75" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C75" s="5">
+      <c r="B75" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C75" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D75" s="5">
         <v>20</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B76" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C76" s="7">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="77" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="B76" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C76" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D76" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B77" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C77" s="11">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="78" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="B77" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C77" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D77" s="4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B78" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C78" s="6">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="79" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="B78" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D78" s="5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B79" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C79" s="8">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="80" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="B79" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D79" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="B80" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C80" s="5">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="81" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="B80" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D80" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B81" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C81" s="6">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="82" spans="1:3" ht="21" x14ac:dyDescent="0.25">
+      <c r="B81" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D81" s="7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" ht="21" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B82" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="C82" s="5">
-        <v>20</v>
+      <c r="B82" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C82" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D82" s="4">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>